<commit_message>
OO-6734: trim teachers names, star for mandatory fields in template
</commit_message>
<xml_diff>
--- a/src/main/resources/org/olat/modules/lecture/ui/blockimport/lecture-block-import-template.xlsx
+++ b/src/main/resources/org/olat/modules/lecture/ui/blockimport/lecture-block-import-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srosse/Developer/Work/ws_branches/OpenOLAT/src/main/resources/org/olat/modules/lecture/ui/blockimport/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8DA54-19C0-E04C-B19B-AE0C152D2A2F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A7296A-D4BF-8D43-9DD4-9537C96EC66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11480" yWindow="5400" windowWidth="35300" windowHeight="13180" xr2:uid="{DB995043-D42B-A34D-A5FC-C5D9B7787277}"/>
   </bookViews>
@@ -27,30 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Lectures</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Start</t>
-  </si>
-  <si>
-    <t>End</t>
-  </si>
-  <si>
-    <t>Compulsory</t>
-  </si>
-  <si>
-    <t>Teacher</t>
-  </si>
-  <si>
-    <t>Participants</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -120,9 +96,6 @@
     <t>L1</t>
   </si>
   <si>
-    <t>External ID</t>
-  </si>
-  <si>
     <t>Teacher identified via user name, Participants from a course group named "Samichlaus"</t>
   </si>
   <si>
@@ -130,6 +103,33 @@
   </si>
   <si>
     <t>Teacher identified via institutional user identifier, participants from a course curriculum element with ID "2018-HS-INFO"</t>
+  </si>
+  <si>
+    <t>External ID*</t>
+  </si>
+  <si>
+    <t>Title*</t>
+  </si>
+  <si>
+    <t>Lectures*</t>
+  </si>
+  <si>
+    <t>Date*</t>
+  </si>
+  <si>
+    <t>Start*</t>
+  </si>
+  <si>
+    <t>End*</t>
+  </si>
+  <si>
+    <t>Compulsory*</t>
+  </si>
+  <si>
+    <t>Teacher*</t>
+  </si>
+  <si>
+    <t>Participants*</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,51 +523,51 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>4</v>
@@ -582,30 +582,30 @@
         <v>0.5</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -620,30 +620,30 @@
         <v>0.875</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -658,22 +658,22 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>12345</v>
       </c>
       <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5" t="s">
         <v>25</v>
-      </c>
-      <c r="J5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M5" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>